<commit_message>
arreglo del incremento del numero de presupuesto
</commit_message>
<xml_diff>
--- a/base_datos.xlsx
+++ b/base_datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CRISTIAN\Mios\mi cotizador\Cotizador-recibos - copia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siste\OneDrive\Escritorio\Nueva carpeta (3)\Cotizador-recibos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13624EB-0670-4A35-801E-2016D45904EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CF365E-896B-4717-A15C-E7EC8E9D371C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -99,9 +99,6 @@
     <t>358-6020639</t>
   </si>
   <si>
-    <t>cpu caja 1</t>
-  </si>
-  <si>
     <t>Mauricio (Giosue)</t>
   </si>
   <si>
@@ -225,12 +222,6 @@
     <t>Hdd 1tb (u)</t>
   </si>
   <si>
-    <t>unidad ssd  240gb (u)</t>
-  </si>
-  <si>
-    <t>unidad ssd  120gb (u)</t>
-  </si>
-  <si>
     <t>Recuperación de sectores de HDD</t>
   </si>
   <si>
@@ -307,6 +298,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>unidad ssd  240gb verico</t>
+  </si>
+  <si>
+    <t>unidad ssd  120gb verico</t>
+  </si>
+  <si>
+    <t>unidad ssd  480gb verico</t>
   </si>
 </sst>
 </file>
@@ -847,11 +847,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
@@ -949,28 +956,26 @@
       <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
         <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -978,19 +983,19 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -998,19 +1003,19 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
         <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1020,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,13 +1049,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1058,10 +1063,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>99</v>
@@ -1075,10 +1080,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3">
         <v>99</v>
@@ -1092,16 +1097,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>99</v>
       </c>
       <c r="E4" s="14">
-        <v>39690</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1109,10 +1114,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>99</v>
@@ -1126,10 +1131,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6">
         <v>99</v>
@@ -1143,10 +1148,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>99</v>
@@ -1160,10 +1165,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>99</v>
@@ -1178,10 +1183,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9">
         <v>99</v>
@@ -1195,10 +1200,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>99</v>
@@ -1212,10 +1217,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11">
         <v>99</v>
@@ -1229,10 +1234,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>99</v>
@@ -1246,10 +1251,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>99</v>
@@ -1263,16 +1268,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14">
         <v>99</v>
       </c>
       <c r="E14" s="14">
-        <v>27000</v>
+        <v>31000</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1280,10 +1285,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>99</v>
@@ -1297,10 +1302,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>99</v>
@@ -1314,10 +1319,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17">
         <v>99</v>
@@ -1331,10 +1336,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18">
         <v>99</v>
@@ -1348,10 +1353,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19">
         <v>99</v>
@@ -1365,10 +1370,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>99</v>
@@ -1382,10 +1387,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21">
         <v>99</v>
@@ -1399,10 +1404,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22">
         <v>99</v>
@@ -1416,10 +1421,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23">
         <v>99</v>
@@ -1433,10 +1438,10 @@
         <v>53</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24">
         <v>99</v>
@@ -1452,10 +1457,10 @@
         <v>54</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25">
         <v>99</v>
@@ -1471,10 +1476,10 @@
         <v>57</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26">
         <v>99</v>
@@ -1490,10 +1495,10 @@
         <v>55</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
+        <v>89</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D27">
         <v>99</v>
@@ -1504,72 +1509,72 @@
       <c r="F27" s="15"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28">
+        <v>38</v>
+      </c>
+      <c r="D28" s="9">
         <v>99</v>
       </c>
       <c r="E28" s="14">
-        <v>20000</v>
+        <v>42000</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
-        <v>59</v>
-      </c>
-      <c r="B29" t="s">
-        <v>66</v>
+        <v>56</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D29">
         <v>99</v>
       </c>
       <c r="E29" s="14">
-        <v>21000</v>
+        <v>20000</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
-        <v>58</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>68</v>
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D30">
         <v>99</v>
       </c>
       <c r="E30" s="14">
-        <v>15000</v>
+        <v>21000</v>
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="10"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="D31">
         <v>99</v>
@@ -1585,118 +1590,137 @@
         <v>60</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32">
         <v>99</v>
       </c>
       <c r="E32" s="14">
-        <v>28000</v>
+        <v>15000</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D33">
         <v>99</v>
       </c>
       <c r="E33" s="14">
-        <v>22200</v>
+        <v>28000</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <v>62</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="D34">
         <v>99</v>
       </c>
       <c r="E34" s="14">
-        <v>11000</v>
+        <v>22200</v>
       </c>
       <c r="F34" s="15"/>
       <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <v>63</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>73</v>
+        <v>62</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D35">
         <v>99</v>
       </c>
       <c r="E35" s="14">
-        <v>45000</v>
+        <v>11000</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D36">
         <v>99</v>
       </c>
       <c r="E36" s="14">
-        <v>10000</v>
+        <v>45000</v>
       </c>
       <c r="F36" s="15"/>
       <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="D37">
         <v>99</v>
       </c>
       <c r="E37" s="14">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="10"/>
     </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>66</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38">
+        <v>99</v>
+      </c>
+      <c r="E38" s="14">
+        <v>11000</v>
+      </c>
+      <c r="F38" s="15"/>
+      <c r="G38" s="10"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C37" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C38" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>LISTA_PROVEE</formula1>
     </dataValidation>
   </dataValidations>
@@ -1731,16 +1755,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
         <v>76</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1748,19 +1772,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E2" s="1">
         <v>3586546525</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1768,19 +1792,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E3" s="3">
         <v>3584268768</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G3" s="3"/>
     </row>
@@ -1789,7 +1813,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1802,7 +1826,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -1815,7 +1839,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1847,19 +1871,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>